<commit_message>
Entered in elapsed time for each completed model - 85 scrUN models done to date
</commit_message>
<xml_diff>
--- a/AllSpecies_SC_output.xlsx
+++ b/AllSpecies_SC_output.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="133">
   <si>
     <t>Species</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>scrUN niter</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -761,18 +764,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -812,76 +815,112 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>357.74349999999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>330.43490000000003</v>
+      </c>
+      <c r="F9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
+      </c>
+      <c r="E10" s="1">
+        <v>315.17259999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -898,12 +937,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -962,100 +1004,166 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>224.4923</v>
+      </c>
+      <c r="F17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>285.065</v>
+      </c>
+      <c r="F18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>338.2878</v>
+      </c>
+      <c r="F19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>354.68610000000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>376.1309</v>
+      </c>
+      <c r="F22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>332.0942</v>
+      </c>
+      <c r="F23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <v>375.3494</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1">
+        <v>342.97379999999998</v>
+      </c>
+      <c r="F26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>276.58319999999998</v>
+      </c>
+      <c r="F27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
+      </c>
+      <c r="E28" s="1">
+        <v>384.14019999999999</v>
+      </c>
+      <c r="F28" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,12 +1180,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1108,260 +1219,428 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <v>262.64600000000002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>216.95840000000001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>271.43360000000001</v>
+      </c>
+      <c r="F35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>160.08279999999999</v>
+      </c>
+      <c r="F36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>200.7971</v>
+      </c>
+      <c r="F37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
       <c r="B38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>338.1816</v>
+      </c>
+      <c r="F38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
       <c r="B40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>345.27519999999998</v>
+      </c>
+      <c r="F41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>382.28960000000001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>365.12389999999999</v>
+      </c>
+      <c r="F44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>316.9289</v>
+      </c>
+      <c r="F45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>357.00439999999998</v>
+      </c>
+      <c r="F46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>179.24549999999999</v>
+      </c>
+      <c r="F47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>241.88</v>
+      </c>
+      <c r="F48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>225.34809999999999</v>
+      </c>
+      <c r="F49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>175.3117</v>
+      </c>
+      <c r="F50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>386.73129999999998</v>
+      </c>
+      <c r="F51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
       <c r="B52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>308.4871</v>
+      </c>
+      <c r="F52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
       <c r="B53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>173.50399999999999</v>
+      </c>
+      <c r="F53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>246.5745</v>
+      </c>
+      <c r="F54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>46</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>316.61900000000003</v>
+      </c>
+      <c r="F55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>65</v>
       </c>
       <c r="B57" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>65</v>
       </c>
       <c r="B58" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>366.62209999999999</v>
+      </c>
+      <c r="F58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
       <c r="B59" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>337.46660000000003</v>
+      </c>
+      <c r="F59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <v>380.02769999999998</v>
+      </c>
+      <c r="F61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <v>328.79340000000002</v>
+      </c>
+      <c r="F62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
       <c r="B64" t="s">
         <v>74</v>
+      </c>
+      <c r="F64" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,12 +1657,18 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>76</v>
+      </c>
+      <c r="E66" s="1">
+        <v>293.55540000000002</v>
+      </c>
+      <c r="F66" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,156 +1700,265 @@
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>65</v>
       </c>
       <c r="B69" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="1">
+        <v>291.1884</v>
+      </c>
+      <c r="F69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>65</v>
       </c>
       <c r="B70" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="1">
+        <v>214.27760000000001</v>
+      </c>
+      <c r="F70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="1">
+        <v>248.791</v>
+      </c>
+      <c r="F71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>65</v>
       </c>
       <c r="B72" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="1">
+        <v>317.43889999999999</v>
+      </c>
+      <c r="F72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>65</v>
       </c>
       <c r="B73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
+        <v>354.50920000000002</v>
+      </c>
+      <c r="F73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>84</v>
       </c>
       <c r="B74" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <v>355.92759999999998</v>
+      </c>
+      <c r="F74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>84</v>
       </c>
       <c r="B75" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>84</v>
       </c>
       <c r="B76" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <v>379.75130000000001</v>
+      </c>
+      <c r="F76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
       <c r="B77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
+        <v>325.31920000000002</v>
+      </c>
+      <c r="F77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
       <c r="B78" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="1"/>
+      <c r="F78" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="1">
+        <v>378.03030000000001</v>
+      </c>
+      <c r="F79" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>84</v>
       </c>
       <c r="B80" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="1">
+        <v>300.40339999999998</v>
+      </c>
+      <c r="F80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>84</v>
       </c>
       <c r="B81" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="1">
+        <v>286.58909999999997</v>
+      </c>
+      <c r="F81" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E82" s="1">
+        <v>358.85939999999999</v>
+      </c>
+      <c r="F82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
       <c r="B83" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E83" s="1">
+        <v>175.26300000000001</v>
+      </c>
+      <c r="F83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="1">
+        <v>271.35160000000002</v>
+      </c>
+      <c r="F84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="1">
+        <v>293.7833</v>
+      </c>
+      <c r="F85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E86" s="1">
+        <v>163.3716</v>
+      </c>
+      <c r="F86" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>84</v>
       </c>
       <c r="B87" t="s">
         <v>98</v>
+      </c>
+      <c r="E87" s="1">
+        <v>264.56040000000002</v>
+      </c>
+      <c r="F87" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,100 +1975,163 @@
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
       <c r="B89" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E89" s="1">
+        <v>251.28800000000001</v>
+      </c>
+      <c r="F89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>84</v>
       </c>
       <c r="B90" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E90" s="1">
+        <v>253.25239999999999</v>
+      </c>
+      <c r="F90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>84</v>
       </c>
       <c r="B91" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E91" s="1">
+        <v>335.20519999999999</v>
+      </c>
+      <c r="F91" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>103</v>
       </c>
       <c r="B92" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E92" s="1">
+        <v>340.44009999999997</v>
+      </c>
+      <c r="F92" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>103</v>
       </c>
       <c r="B93" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>103</v>
       </c>
       <c r="B94" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E94" s="1">
+        <v>388.46449999999999</v>
+      </c>
+      <c r="F94" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>103</v>
       </c>
       <c r="B95" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E95" s="1">
+        <v>346.63040000000001</v>
+      </c>
+      <c r="F95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
       <c r="B96" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
       <c r="B97" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E97" s="1">
+        <v>373.16969999999998</v>
+      </c>
+      <c r="F97" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
       <c r="B98" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E98" s="1">
+        <v>303.4726</v>
+      </c>
+      <c r="F98" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>103</v>
       </c>
       <c r="B99" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E99" s="1">
+        <v>286.06790000000001</v>
+      </c>
+      <c r="F99" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>103</v>
       </c>
       <c r="B100" t="s">
         <v>112</v>
+      </c>
+      <c r="F100" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -1691,20 +2148,32 @@
         <v>122</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>103</v>
       </c>
       <c r="B102" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E102" s="1">
+        <v>265.88350000000003</v>
+      </c>
+      <c r="F102" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
       <c r="B103" t="s">
         <v>115</v>
+      </c>
+      <c r="E103" s="1">
+        <v>301.32100000000003</v>
+      </c>
+      <c r="F103" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -1721,12 +2190,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>117</v>
+      </c>
+      <c r="F105" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,38 +2215,56 @@
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
       <c r="B107" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E107" s="1">
+        <v>285.50830000000002</v>
+      </c>
+      <c r="F107" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>103</v>
       </c>
       <c r="B108" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E108" s="1">
+        <v>262.3295</v>
+      </c>
+      <c r="F108" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>103</v>
       </c>
       <c r="B109" t="s">
         <v>121</v>
       </c>
+      <c r="E109" s="1">
+        <v>355.07299999999998</v>
+      </c>
+      <c r="F109" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <f>283.4/24</f>
+        <v>11.808333333333332</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K109">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K109"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>